<commit_message>
Add new column (Duration)
</commit_message>
<xml_diff>
--- a/problems_types.xlsx
+++ b/problems_types.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC10504-7F02-4838-8A70-8B51BABBAF19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="types" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>type</t>
   </si>
@@ -43,12 +44,15 @@
   </si>
   <si>
     <t>Flickering light</t>
+  </si>
+  <si>
+    <t>duration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,8 +82,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,57 +366,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="75.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="75.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="1">
+        <v>60</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" s="1">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" s="1">
+        <v>40</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>